<commit_message>
Replicando analisis en JASP
</commit_message>
<xml_diff>
--- a/Datos/JASP_Datos_subjuego1_r3.xlsx
+++ b/Datos/JASP_Datos_subjuego1_r3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Sesion</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>TC</t>
+  </si>
+  <si>
+    <t>Dan</t>
   </si>
 </sst>
 </file>
@@ -883,11 +886,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
-      <selection activeCell="CA8" sqref="CA8"/>
+    <sheetView tabSelected="1" topLeftCell="BY1" workbookViewId="0">
+      <selection activeCell="CU21" sqref="CU21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="90" max="90" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1157,7 +1163,9 @@
       <c r="CK1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" s="25"/>
+      <c r="CL1" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="2" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -1421,7 +1429,10 @@
       <c r="CI2" s="25"/>
       <c r="CJ2" s="25"/>
       <c r="CK2" s="25"/>
-      <c r="CL2" s="25"/>
+      <c r="CL2" s="25">
+        <f>AVERAGE(V2,AT2,BR2)</f>
+        <v>-0.45813953488372089</v>
+      </c>
     </row>
     <row r="3" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1685,7 +1696,10 @@
       <c r="CI3" s="25"/>
       <c r="CJ3" s="25"/>
       <c r="CK3" s="25"/>
-      <c r="CL3" s="25"/>
+      <c r="CL3" s="25">
+        <f t="shared" ref="CL3:CL37" si="0">AVERAGE(V3,AT3,BR3)</f>
+        <v>-5.5084745762711849E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1949,7 +1963,10 @@
       <c r="CI4" s="25"/>
       <c r="CJ4" s="25"/>
       <c r="CK4" s="25"/>
-      <c r="CL4" s="25"/>
+      <c r="CL4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.65254237288135586</v>
+      </c>
     </row>
     <row r="5" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2219,7 +2236,10 @@
       <c r="CK5" s="25">
         <v>13</v>
       </c>
-      <c r="CL5" s="25"/>
+      <c r="CL5" s="25">
+        <f t="shared" si="0"/>
+        <v>1.6216216216216217</v>
+      </c>
     </row>
     <row r="6" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -2483,7 +2503,10 @@
       <c r="CI6" s="25"/>
       <c r="CJ6" s="25"/>
       <c r="CK6" s="25"/>
-      <c r="CL6" s="25"/>
+      <c r="CL6" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.18351063829787231</v>
+      </c>
     </row>
     <row r="7" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -2747,7 +2770,10 @@
       <c r="CI7" s="25"/>
       <c r="CJ7" s="25"/>
       <c r="CK7" s="25"/>
-      <c r="CL7" s="25"/>
+      <c r="CL7" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.29197080291970806</v>
+      </c>
     </row>
     <row r="8" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -3011,7 +3037,10 @@
       <c r="CI8" s="25"/>
       <c r="CJ8" s="25"/>
       <c r="CK8" s="25"/>
-      <c r="CL8" s="25"/>
+      <c r="CL8" s="25">
+        <f t="shared" si="0"/>
+        <v>6.5384615384615388E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -3281,7 +3310,10 @@
       <c r="CK9" s="25">
         <v>5</v>
       </c>
-      <c r="CL9" s="25"/>
+      <c r="CL9" s="25">
+        <f t="shared" si="0"/>
+        <v>0.30645161290322581</v>
+      </c>
     </row>
     <row r="10" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -3545,7 +3577,10 @@
       <c r="CI10" s="25"/>
       <c r="CJ10" s="25"/>
       <c r="CK10" s="25"/>
-      <c r="CL10" s="25"/>
+      <c r="CL10" s="25">
+        <f t="shared" si="0"/>
+        <v>0.69444444444444431</v>
+      </c>
     </row>
     <row r="11" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -3809,7 +3844,10 @@
       <c r="CI11" s="25"/>
       <c r="CJ11" s="25"/>
       <c r="CK11" s="25"/>
-      <c r="CL11" s="25"/>
+      <c r="CL11" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.2608695652173913</v>
+      </c>
     </row>
     <row r="12" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -4073,7 +4111,10 @@
       <c r="CI12" s="25"/>
       <c r="CJ12" s="25"/>
       <c r="CK12" s="25"/>
-      <c r="CL12" s="25"/>
+      <c r="CL12" s="25">
+        <f t="shared" si="0"/>
+        <v>0.1328125</v>
+      </c>
     </row>
     <row r="13" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -4343,7 +4384,10 @@
       <c r="CK13" s="25">
         <v>1</v>
       </c>
-      <c r="CL13" s="25"/>
+      <c r="CL13" s="25">
+        <f t="shared" si="0"/>
+        <v>0.38461538461538464</v>
+      </c>
     </row>
     <row r="14" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -4607,7 +4651,10 @@
       <c r="CI14" s="25"/>
       <c r="CJ14" s="25"/>
       <c r="CK14" s="25"/>
-      <c r="CL14" s="25"/>
+      <c r="CL14" s="25">
+        <f t="shared" si="0"/>
+        <v>-6.3291139240506666E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -4871,7 +4918,10 @@
       <c r="CI15" s="25"/>
       <c r="CJ15" s="25"/>
       <c r="CK15" s="25"/>
-      <c r="CL15" s="25"/>
+      <c r="CL15" s="25">
+        <f t="shared" si="0"/>
+        <v>0.46470588235294125</v>
+      </c>
     </row>
     <row r="16" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -5135,7 +5185,10 @@
       <c r="CI16" s="25"/>
       <c r="CJ16" s="25"/>
       <c r="CK16" s="25"/>
-      <c r="CL16" s="25"/>
+      <c r="CL16" s="25">
+        <f t="shared" si="0"/>
+        <v>0.19607843137254899</v>
+      </c>
     </row>
     <row r="17" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -5405,7 +5458,10 @@
       <c r="CK17" s="25">
         <v>3</v>
       </c>
-      <c r="CL17" s="25"/>
+      <c r="CL17" s="25">
+        <f t="shared" si="0"/>
+        <v>0.81818181818181834</v>
+      </c>
     </row>
     <row r="18" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -5669,7 +5725,10 @@
       <c r="CI18" s="25"/>
       <c r="CJ18" s="25"/>
       <c r="CK18" s="25"/>
-      <c r="CL18" s="25"/>
+      <c r="CL18" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.9736842105263146E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -5933,7 +5992,10 @@
       <c r="CI19" s="25"/>
       <c r="CJ19" s="25"/>
       <c r="CK19" s="25"/>
-      <c r="CL19" s="25"/>
+      <c r="CL19" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.34090909090909088</v>
+      </c>
     </row>
     <row r="20" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -6197,7 +6259,10 @@
       <c r="CI20" s="25"/>
       <c r="CJ20" s="25"/>
       <c r="CK20" s="25"/>
-      <c r="CL20" s="25"/>
+      <c r="CL20" s="25">
+        <f t="shared" si="0"/>
+        <v>-9.4488188976377938E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -6467,7 +6532,10 @@
       <c r="CK21" s="25">
         <v>9</v>
       </c>
-      <c r="CL21" s="25"/>
+      <c r="CL21" s="25">
+        <f t="shared" si="0"/>
+        <v>0.25714285714285717</v>
+      </c>
     </row>
     <row r="22" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -6731,7 +6799,10 @@
       <c r="CI22" s="25"/>
       <c r="CJ22" s="25"/>
       <c r="CK22" s="25"/>
-      <c r="CL22" s="25"/>
+      <c r="CL22" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.18897637795275588</v>
+      </c>
     </row>
     <row r="23" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -6995,7 +7066,10 @@
       <c r="CI23" s="25"/>
       <c r="CJ23" s="25"/>
       <c r="CK23" s="25"/>
-      <c r="CL23" s="25"/>
+      <c r="CL23" s="25">
+        <f t="shared" si="0"/>
+        <v>7.9207920792079237E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -7259,7 +7333,10 @@
       <c r="CI24" s="25"/>
       <c r="CJ24" s="25"/>
       <c r="CK24" s="25"/>
-      <c r="CL24" s="25"/>
+      <c r="CL24" s="25">
+        <f t="shared" si="0"/>
+        <v>1.6888888888888889</v>
+      </c>
     </row>
     <row r="25" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -7529,7 +7606,10 @@
       <c r="CK25" s="25">
         <v>13</v>
       </c>
-      <c r="CL25" s="25"/>
+      <c r="CL25" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.19626168224299065</v>
+      </c>
     </row>
     <row r="26" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -7793,7 +7873,10 @@
       <c r="CI26" s="25"/>
       <c r="CJ26" s="25"/>
       <c r="CK26" s="25"/>
-      <c r="CL26" s="25"/>
+      <c r="CL26" s="25">
+        <f t="shared" si="0"/>
+        <v>0.73529411764705888</v>
+      </c>
     </row>
     <row r="27" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -8057,7 +8140,10 @@
       <c r="CI27" s="25"/>
       <c r="CJ27" s="25"/>
       <c r="CK27" s="25"/>
-      <c r="CL27" s="25"/>
+      <c r="CL27" s="25">
+        <f t="shared" si="0"/>
+        <v>-2.5000000000000005E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -8321,7 +8407,10 @@
       <c r="CI28" s="25"/>
       <c r="CJ28" s="25"/>
       <c r="CK28" s="25"/>
-      <c r="CL28" s="25"/>
+      <c r="CL28" s="25">
+        <f t="shared" si="0"/>
+        <v>4.301075268817204E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -8591,7 +8680,10 @@
       <c r="CK29" s="25">
         <v>8</v>
       </c>
-      <c r="CL29" s="25"/>
+      <c r="CL29" s="25">
+        <f t="shared" si="0"/>
+        <v>-3.6585365853658534E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -8855,7 +8947,10 @@
       <c r="CI30" s="25"/>
       <c r="CJ30" s="25"/>
       <c r="CK30" s="25"/>
-      <c r="CL30" s="25"/>
+      <c r="CL30" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.53424657534246578</v>
+      </c>
     </row>
     <row r="31" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -9119,7 +9214,10 @@
       <c r="CI31" s="25"/>
       <c r="CJ31" s="25"/>
       <c r="CK31" s="25"/>
-      <c r="CL31" s="25"/>
+      <c r="CL31" s="25">
+        <f t="shared" si="0"/>
+        <v>0.11792452830188678</v>
+      </c>
     </row>
     <row r="32" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -9383,7 +9481,10 @@
       <c r="CI32" s="25"/>
       <c r="CJ32" s="25"/>
       <c r="CK32" s="25"/>
-      <c r="CL32" s="25"/>
+      <c r="CL32" s="25">
+        <f t="shared" si="0"/>
+        <v>-1.9607843137254902E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -9653,7 +9754,10 @@
       <c r="CK33" s="25">
         <v>3</v>
       </c>
-      <c r="CL33" s="25"/>
+      <c r="CL33" s="25">
+        <f t="shared" si="0"/>
+        <v>1.5957446808510634E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -9917,7 +10021,10 @@
       <c r="CI34" s="25"/>
       <c r="CJ34" s="25"/>
       <c r="CK34" s="25"/>
-      <c r="CL34" s="25"/>
+      <c r="CL34" s="25">
+        <f t="shared" si="0"/>
+        <v>-0.265625</v>
+      </c>
     </row>
     <row r="35" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -10181,7 +10288,10 @@
       <c r="CI35" s="25"/>
       <c r="CJ35" s="25"/>
       <c r="CK35" s="25"/>
-      <c r="CL35" s="25"/>
+      <c r="CL35" s="25">
+        <f t="shared" si="0"/>
+        <v>0.11607142857142856</v>
+      </c>
     </row>
     <row r="36" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -10445,7 +10555,10 @@
       <c r="CI36" s="25"/>
       <c r="CJ36" s="25"/>
       <c r="CK36" s="25"/>
-      <c r="CL36" s="25"/>
+      <c r="CL36" s="25">
+        <f t="shared" si="0"/>
+        <v>0.11363636363636365</v>
+      </c>
     </row>
     <row r="37" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -10715,7 +10828,10 @@
       <c r="CK37" s="25">
         <v>12</v>
       </c>
-      <c r="CL37" s="25"/>
+      <c r="CL37" s="25">
+        <f t="shared" si="0"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>